<commit_message>
added headers to the 20 counter sheet for verification req
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010371\Documents\VHDL Training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/my_repos/Verilog_Stopwatch/Life_Cycle_Data/Requirements_Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84224FAB-1016-4CD7-8A92-CB1E6AC9DF71}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E0ACFE-0FA7-634A-A852-368ED78502F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Initialization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Requirement Header </t>
   </si>
 </sst>
 </file>
@@ -433,20 +436,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B4EAFD-D6BC-4B33-AEA7-1FB008F58338}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="71.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -463,7 +466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -480,7 +483,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" s="3"/>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -503,7 +506,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -511,12 +514,39 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2C20F1-AFF3-4389-955F-F90E6A0B5D40}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -527,7 +557,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -539,13 +569,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11c68bd7e868490b50c80001f2cf6c52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" xmlns:ns3="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7feae6b8f12256f9c4998c90aa2e28a" ns2:_="" ns3:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -724,29 +769,38 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
+    <ds:schemaRef ds:uri="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Merged the Excel Docs
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colinfritz/my_repos/Verilog_Stopwatch/Life_Cycle_Data/Requirements_Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Documents\GitHub\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4E0ACFE-0FA7-634A-A852-368ED78502F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9AB576-11E7-4ACB-943D-F15CB3967C2D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Trigger Detection" sheetId="1" r:id="rId1"/>
+    <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
     <sheet name="10ms Timer" sheetId="2" r:id="rId2"/>
-    <sheet name="20-Bit Counter" sheetId="3" r:id="rId3"/>
-    <sheet name="7-Seg Decoder" sheetId="4" r:id="rId4"/>
+    <sheet name="20-Bit BCD Counter" sheetId="3" r:id="rId3"/>
+    <sheet name="20-bit BCD to 7-Segment Display" sheetId="4" r:id="rId4"/>
     <sheet name="General" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -71,6 +71,75 @@
   </si>
   <si>
     <t>Initialization</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout1 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout2 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout3 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout4 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout5 to "1111111" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout1 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout2 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout3 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout4 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segout5 to "1111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>DRV</t>
+  </si>
+  <si>
+    <t>DRV_INIT_01</t>
+  </si>
+  <si>
+    <t>DRV_INIT_02</t>
+  </si>
+  <si>
+    <t>DRV_INIT_03</t>
+  </si>
+  <si>
+    <t>DRV_INIT_04</t>
+  </si>
+  <si>
+    <t>DRV_INIT_05</t>
+  </si>
+  <si>
+    <t>DRV_INIT_06</t>
+  </si>
+  <si>
+    <t>DRV_INIT_07</t>
+  </si>
+  <si>
+    <t>DRV_INIT_08</t>
+  </si>
+  <si>
+    <t>DRV_INIT_09</t>
+  </si>
+  <si>
+    <t>DRV_INIT_10</t>
+  </si>
+  <si>
+    <t>DRV_MAP_01</t>
+  </si>
+  <si>
+    <t>BCD to 7-segment mapping</t>
   </si>
   <si>
     <t xml:space="preserve">Requirement Header </t>
@@ -80,10 +149,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -97,7 +172,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -105,11 +180,124 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -117,7 +305,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -436,20 +652,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B4EAFD-D6BC-4B33-AEA7-1FB008F58338}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -466,14 +682,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -483,8 +699,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="3"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="10"/>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
@@ -506,7 +722,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -514,35 +730,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2C20F1-AFF3-4389-955F-F90E6A0B5D40}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -553,12 +765,145 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B94154-4E96-428E-BDF1-A1ABE2650270}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="12"/>
+      <c r="C4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="12"/>
+      <c r="C5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="12"/>
+      <c r="C6" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="12"/>
+      <c r="C7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="12"/>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="12"/>
+      <c r="C9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="12"/>
+      <c r="C10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="13"/>
+      <c r="C11" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:B11"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -569,28 +914,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11c68bd7e868490b50c80001f2cf6c52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" xmlns:ns3="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7feae6b8f12256f9c4998c90aa2e28a" ns2:_="" ns3:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -769,24 +1099,22 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -803,4 +1131,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[SWATCH2-21] + [SWATCH2-146] andrew-7seg-reqs-done
[SWATCH2-146] Completed the FPGA adapter requirements.
[SWATCH2-21] Resubmitting the requirements due to no outstanding changes in system specifications.

To be reviewed by @colinfritzltts .
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Documents\GitHub\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB0D2696-368E-41E1-A829-E18634D5DB0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A2E6AC-9039-4D1D-9496-707E57FB111A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
     <sheet name="10ms Timer" sheetId="2" r:id="rId2"/>
     <sheet name="20-Bit BCD Counter" sheetId="3" r:id="rId3"/>
     <sheet name="20-bit BCD to 7-Segment Display" sheetId="4" r:id="rId4"/>
-    <sheet name="General" sheetId="5" r:id="rId5"/>
+    <sheet name="7-Segment FPGA Adapter" sheetId="6" r:id="rId5"/>
+    <sheet name="General" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="223">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -79,21 +80,6 @@
     <t>DRV_INIT_05</t>
   </si>
   <si>
-    <t>DRV_INIT_06</t>
-  </si>
-  <si>
-    <t>DRV_INIT_07</t>
-  </si>
-  <si>
-    <t>DRV_INIT_08</t>
-  </si>
-  <si>
-    <t>DRV_INIT_09</t>
-  </si>
-  <si>
-    <t>DRV_INIT_10</t>
-  </si>
-  <si>
     <t xml:space="preserve">Requirement Header </t>
   </si>
   <si>
@@ -181,9 +167,6 @@
     <t>TDC_FSM_03</t>
   </si>
   <si>
-    <t>Initialization and Reset conditions</t>
-  </si>
-  <si>
     <t>The module shall preset o_segout1 to "11111111" upon system startup.</t>
   </si>
   <si>
@@ -199,30 +182,12 @@
     <t>The module shall preset o_segout5 to "11111111" upon system startup.</t>
   </si>
   <si>
-    <t>The module shall set o_segout1 to "11111111" when i_reset_n is set to logic low.</t>
-  </si>
-  <si>
-    <t>The module shall set o_segout2 to "11111111" when i_reset_n is set to logic low.</t>
-  </si>
-  <si>
-    <t>The module shall set o_segout3 to "11111111" when i_reset_n is set to logic low.</t>
-  </si>
-  <si>
-    <t>The module shall set o_segout4 to "11111111" when i_reset_n is set to logic low.</t>
-  </si>
-  <si>
-    <t>The module shall set o_segout5 to "11111111" when i_reset_n is set to logic low.</t>
-  </si>
-  <si>
     <t>Mapping o_segout1</t>
   </si>
   <si>
     <t>DRV_MAP1_01</t>
   </si>
   <si>
-    <t>The module shall append the DRV_MAP1_ group of requirements to the module's intialized value of o_segout1 on a rising edge of i_sclk.</t>
-  </si>
-  <si>
     <t>DRV_MAP1_02</t>
   </si>
   <si>
@@ -277,9 +242,6 @@
     <t>DRV_MAP2_01</t>
   </si>
   <si>
-    <t>The module shall append the DRV_MAP2_ group of requirements to the module's intialized value of o_segout2 on a rising edge of i_sclk.</t>
-  </si>
-  <si>
     <t>DRV_MAP2_02</t>
   </si>
   <si>
@@ -334,9 +296,6 @@
     <t>DRV_MAP3_01</t>
   </si>
   <si>
-    <t>The module shall append the DRV_MAP3_ group of requirements to the module's intialized value of o_segout3 on a rising edge of i_sclk.</t>
-  </si>
-  <si>
     <t>DRV_MAP3_02</t>
   </si>
   <si>
@@ -391,9 +350,6 @@
     <t>DRV_MAP4_01</t>
   </si>
   <si>
-    <t>The module shall append the DRV_MAP4_ group of requirements to the module's intialized value of o_segout4 on a rising edge of i_sclk.</t>
-  </si>
-  <si>
     <t>DRV_MAP4_02</t>
   </si>
   <si>
@@ -448,9 +404,6 @@
     <t>DRV_MAP5_01</t>
   </si>
   <si>
-    <t>The module shall append the DRV_MAP5_ group of requirements to the module's intialized value of o_segout5 on a rising edge of i_sclk.</t>
-  </si>
-  <si>
     <t>DRV_MAP5_02</t>
   </si>
   <si>
@@ -497,6 +450,261 @@
   </si>
   <si>
     <t>The module shall set o_segout5[0] to logic low when i_count[19:16] is set to "0010" or "0011" or "0100" or "0101" or "0110" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>Mapping o_segout6</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_01</t>
+  </si>
+  <si>
+    <t>The module shall append the DRV_MAP4_ group of requirements to the module's intialized value of o_segout4.</t>
+  </si>
+  <si>
+    <t>The module shall append the DRV_MAP5_ group of requirements to the module's intialized value of o_segout5.</t>
+  </si>
+  <si>
+    <t>The module shall append the DRV_MAP3_ group of requirements to the module's intialized value of o_segout3.</t>
+  </si>
+  <si>
+    <t>The module shall append the DRV_MAP2_ group of requirements to the module's intialized value of o_segout2.</t>
+  </si>
+  <si>
+    <t>The module shall append the DRV_MAP1_ group of requirements to the module's intialized value of o_segout1.</t>
+  </si>
+  <si>
+    <t>The module shall append the DRV_MAP6_ group of requirements to the module's intialized value of o_segout6.</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_02</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_03</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_04</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_05</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_06</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_07</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_08</t>
+  </si>
+  <si>
+    <t>DRV_MAP6_09</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[7] to logic low when i_count[23:20] is set to "0001" or "0011" or "0101" or "0111" or "1001".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[6] to logic low when i_count[23:20] is set to "0000" or "0010" or "0011" or "0101" or "0110" or "0111" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[5] to logic low when i_count[23:20] is set to "0000" or "0001" or "0010" or "0011" or "0100" or "0111" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[4] to logic low when i_count[23:20] is set to "0000" or "0001" or "0011" or "0100" or "0101" or "0110" or "0111" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[3] to logic low when i_count[23:20] is set to "0000" or "0010" or "0111" or "0101" or "0110" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[2] to logic low when i_count[23:20] is set to "0000" or "0010" or "0110" or "1000".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[1] to logic low when i_count[23:20] is set to "0000" or "0100" or "0101" or "0110" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>The module shall set o_segout6[0] to logic low when i_count[23:20] is set to "0010" or "0011" or "0100" or "0101" or "0110" or "1000" or "1001".</t>
+  </si>
+  <si>
+    <t>FPGA</t>
+  </si>
+  <si>
+    <t>Initialization and Reset</t>
+  </si>
+  <si>
+    <t>The module shall preset o_segments to "11111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset o_digits to "11111111" upon system startup.</t>
+  </si>
+  <si>
+    <t>FPGA_INIT_01</t>
+  </si>
+  <si>
+    <t>FPGA_INIT_02</t>
+  </si>
+  <si>
+    <t>FPGA_DIV_01</t>
+  </si>
+  <si>
+    <t>FPGA_DIV_02</t>
+  </si>
+  <si>
+    <t>The module shall generate an internal clock signal intclk with period of 1ms based on clock division of i_sclk.</t>
+  </si>
+  <si>
+    <t>The module shall set intclk to a falling edge when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>1-millisecond Clock Divider for Digit Frame</t>
+  </si>
+  <si>
+    <t>Digit Frame FSM</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_01</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_02</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_03</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_04</t>
+  </si>
+  <si>
+    <t>The module shall set internal state intstate to FRM1 when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall set intstate equal to intstatenext on rising edge of intclk. </t>
+  </si>
+  <si>
+    <t>The module shall set intstatenext equal to FRM1 when intstate is equal to FRM6.</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_05</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_06</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_07</t>
+  </si>
+  <si>
+    <t>FPGA_FSM_08</t>
+  </si>
+  <si>
+    <t>The module shall set intstatenext equal to FRM2 when intstate is equal to FRM1.</t>
+  </si>
+  <si>
+    <t>The module shall set intstatenext equal to FRM3 when intstate is equal to FRM2.</t>
+  </si>
+  <si>
+    <t>The module shall set intstatenext equal to FRM4 when intstate is equal to FRM3.</t>
+  </si>
+  <si>
+    <t>The module shall set intstatenext equal to FRM5 when intstate is equal to FRM4.</t>
+  </si>
+  <si>
+    <t>The module shall set intstatenext equal to FRM6 when intstate is equal to FRM5.</t>
+  </si>
+  <si>
+    <t>FPGA_INIT_03</t>
+  </si>
+  <si>
+    <t>FPGA_INIT_04</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_01</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_02</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to i_segout1 when intstate is equal to FRM1.</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_03</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_04</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_05</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_06</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to i_segout6 when intstate is equal to FRM6.</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to i_segout5 when intstate is equal to FRM5.</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to i_segout4 when intstate is equal to FRM4.</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to i_segout3 when intstate is equal to FRM3.</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to i_segout2 when intstate is equal to FRM2.</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_07</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_08</t>
+  </si>
+  <si>
+    <t>The module shall set o_digits equal to "00000000" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "00000000" when i_reset_n is set to logic low.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "11111110" when intstate is equal to FRM1.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "11011111" when intstate is equal to FRM6.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "11101111" when intstate is equal to FRM5.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "11110111" when intstate is equal to FRM4.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "11111011" when intstate is equal to FRM3.</t>
+  </si>
+  <si>
+    <t>The module shall set o_segments equal to "11111101" when intstate is equal to FRM2.</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_09</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_10</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_11</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_12</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_13</t>
+  </si>
+  <si>
+    <t>FPGA_OUT_14</t>
+  </si>
+  <si>
+    <t>The module shall preset intstatenext equal to FRM1 upon system startup.</t>
+  </si>
+  <si>
+    <t>The module shall preset intstate equal to FRM6 upon system startup.</t>
+  </si>
+  <si>
+    <t>Output Manipulation</t>
   </si>
 </sst>
 </file>
@@ -539,7 +747,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -952,17 +1160,45 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -977,84 +1213,32 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1100,7 +1284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1178,27 +1362,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1214,55 +1415,79 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1581,7 +1806,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B11"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,151 +1832,151 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="52" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="20" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
       <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="50"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="50"/>
+      <c r="B12" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="50"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="51"/>
+      <c r="C15" s="16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="11" t="s">
+      <c r="D15" s="17" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="43"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,7 +2061,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -1855,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6B94154-4E96-428E-BDF1-A1ABE2650270}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48:B56"/>
+    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C60" activeCellId="3" sqref="C54 C56 C58 C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1885,579 +2110,622 @@
       </c>
       <c r="E1" s="32"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="57"/>
+      <c r="C3" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
+      <c r="B4" s="57"/>
+      <c r="C4" s="43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="59"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="59"/>
+      <c r="B6" s="57"/>
+      <c r="C6" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="59"/>
+      <c r="B7" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="51" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="48"/>
-      <c r="B3" s="60"/>
-      <c r="C3" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="53" t="s">
+      <c r="D7" s="34" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="59"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="43" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="48"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="35" t="s">
+      <c r="D8" s="44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="48"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="52" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="53" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="48"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="35" t="s">
+      <c r="D9" s="35" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="48"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="52" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="53" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="43" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="35" t="s">
+      <c r="D10" s="46" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="53" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+      <c r="B11" s="62"/>
+      <c r="C11" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="35" t="s">
+      <c r="D11" s="36" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="55" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="43" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="48"/>
-      <c r="B12" s="62" t="s">
+      <c r="D12" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="33" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D13" s="36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="48"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="52" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D14" s="46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="48"/>
-      <c r="B14" s="63"/>
-      <c r="C14" s="2" t="s">
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="59"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D15" s="37" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="48"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="52" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="C16" s="42" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="48"/>
-      <c r="B16" s="63"/>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="47" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="36" t="s">
+      <c r="D17" s="35" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="52" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="59"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D18" s="44" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="2" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D18" s="36" t="s">
+      <c r="D19" s="36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="48"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="52" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="D19" s="56" t="s">
+      <c r="D20" s="46" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="3" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="37" t="s">
+      <c r="D21" s="36" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="62" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="50" t="s">
+      <c r="D22" s="46" t="s">
         <v>79</v>
       </c>
-      <c r="D21" s="57" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="2" t="s">
+      <c r="D23" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="D22" s="35" t="s">
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="59"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="45" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="52" t="s">
+      <c r="D24" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="53" t="s">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="61" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="2" t="s">
+      <c r="C25" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="36" t="s">
+      <c r="D25" s="39" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="59"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="43" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="52" t="s">
+      <c r="D26" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D25" s="56" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="59"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="2" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="2" t="s">
+      <c r="D27" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D26" s="36" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="43" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="52" t="s">
+      <c r="D28" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="56" t="s">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="59"/>
+      <c r="B29" s="62"/>
+      <c r="C29" s="2" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="2" t="s">
+      <c r="D29" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="36" t="s">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="59"/>
+      <c r="B30" s="62"/>
+      <c r="C30" s="43" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48"/>
-      <c r="B29" s="64"/>
-      <c r="C29" s="54" t="s">
+      <c r="D30" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="58" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="59"/>
+      <c r="B31" s="62"/>
+      <c r="C31" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="63" t="s">
+      <c r="D31" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="C30" s="38" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="59"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D30" s="39" t="s">
+      <c r="D32" s="46" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="52" t="s">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="59"/>
+      <c r="B33" s="63"/>
+      <c r="C33" s="40" t="s">
         <v>100</v>
       </c>
-      <c r="D31" s="53" t="s">
+      <c r="D33" s="41" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="2" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="59"/>
+      <c r="B34" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="C34" s="42" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="52" t="s">
+      <c r="D34" s="47" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="59"/>
+      <c r="B35" s="62"/>
+      <c r="C35" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="D35" s="35" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="2" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="59"/>
+      <c r="B36" s="62"/>
+      <c r="C36" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="D34" s="36" t="s">
+      <c r="D36" s="44" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="52" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="59"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="D37" s="36" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="2" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="59"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="D36" s="36" t="s">
+      <c r="D38" s="46" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="48"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="52" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="59"/>
+      <c r="B39" s="62"/>
+      <c r="C39" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D37" s="56" t="s">
+      <c r="D39" s="36" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="48"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="59"/>
+      <c r="B40" s="62"/>
+      <c r="C40" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="D38" s="41" t="s">
+      <c r="D40" s="46" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
-      <c r="B39" s="62" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="59"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="50" t="s">
+      <c r="D41" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="D39" s="57" t="s">
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="59"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="45" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="2" t="s">
+      <c r="D42" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="35" t="s">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="59"/>
+      <c r="B43" s="61" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
-      <c r="B41" s="63"/>
-      <c r="C41" s="52" t="s">
+      <c r="C43" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="53" t="s">
+      <c r="D43" s="39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="59"/>
+      <c r="B44" s="62"/>
+      <c r="C44" s="43" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="63"/>
-      <c r="C42" s="2" t="s">
+      <c r="D44" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="36" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="59"/>
+      <c r="B45" s="62"/>
+      <c r="C45" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
-      <c r="B43" s="63"/>
-      <c r="C43" s="52" t="s">
+      <c r="D45" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="56" t="s">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="59"/>
+      <c r="B46" s="62"/>
+      <c r="C46" s="43" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
-      <c r="B44" s="63"/>
-      <c r="C44" s="2" t="s">
+      <c r="D46" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="36" t="s">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="59"/>
+      <c r="B47" s="62"/>
+      <c r="C47" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="48"/>
-      <c r="B45" s="63"/>
-      <c r="C45" s="52" t="s">
+      <c r="D47" s="36" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="56" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="59"/>
+      <c r="B48" s="62"/>
+      <c r="C48" s="43" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="48"/>
-      <c r="B46" s="63"/>
-      <c r="C46" s="2" t="s">
+      <c r="D48" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="D46" s="36" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="59"/>
+      <c r="B49" s="62"/>
+      <c r="C49" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="48"/>
-      <c r="B47" s="64"/>
-      <c r="C47" s="54" t="s">
+      <c r="D49" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="D47" s="58" t="s">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="59"/>
+      <c r="B50" s="62"/>
+      <c r="C50" s="43" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="48"/>
-      <c r="B48" s="63" t="s">
+      <c r="D50" s="46" t="s">
         <v>135</v>
       </c>
-      <c r="C48" s="38" t="s">
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="59"/>
+      <c r="B51" s="63"/>
+      <c r="C51" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="D48" s="39" t="s">
+      <c r="D51" s="37" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="48"/>
-      <c r="B49" s="63"/>
-      <c r="C49" s="52" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="59"/>
+      <c r="B52" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="D49" s="53" t="s">
+      <c r="C52" s="42" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="48"/>
-      <c r="B50" s="63"/>
-      <c r="C50" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="D50" s="35" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="48"/>
-      <c r="B51" s="63"/>
-      <c r="C51" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="D51" s="56" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="48"/>
-      <c r="B52" s="63"/>
-      <c r="C52" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="D52" s="36" t="s">
+      <c r="D52" s="47" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="48"/>
-      <c r="B53" s="63"/>
-      <c r="C53" s="52" t="s">
+      <c r="A53" s="59"/>
+      <c r="B53" s="62"/>
+      <c r="C53" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="56" t="s">
+      <c r="D53" s="35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="59"/>
+      <c r="B54" s="62"/>
+      <c r="C54" s="43" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="48"/>
-      <c r="B54" s="63"/>
-      <c r="C54" s="2" t="s">
+      <c r="D54" s="44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="59"/>
+      <c r="B55" s="62"/>
+      <c r="C55" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D54" s="36" t="s">
+      <c r="D55" s="36" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="59"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="43" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="48"/>
-      <c r="B55" s="63"/>
-      <c r="C55" s="52" t="s">
+      <c r="D56" s="46" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="59"/>
+      <c r="B57" s="62"/>
+      <c r="C57" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D55" s="56" t="s">
+      <c r="D57" s="36" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="59"/>
+      <c r="B58" s="62"/>
+      <c r="C58" s="43" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="49"/>
-      <c r="B56" s="64"/>
-      <c r="C56" s="3" t="s">
+      <c r="D58" s="46" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="59"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="37" t="s">
+      <c r="D59" s="36" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="60"/>
+      <c r="B60" s="63"/>
+      <c r="C60" s="45" t="s">
         <v>153</v>
       </c>
+      <c r="D60" s="48" t="s">
+        <v>161</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B2:B11"/>
-    <mergeCell ref="A2:A56"/>
-    <mergeCell ref="B12:B20"/>
-    <mergeCell ref="B21:B29"/>
-    <mergeCell ref="B30:B38"/>
-    <mergeCell ref="B39:B47"/>
-    <mergeCell ref="B48:B56"/>
+  <mergeCells count="8">
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A2:A60"/>
+    <mergeCell ref="B7:B15"/>
+    <mergeCell ref="B16:B24"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="B34:B42"/>
+    <mergeCell ref="B43:B51"/>
+    <mergeCell ref="B52:B60"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2465,6 +2733,537 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98609ECE-6D72-4BF1-85BE-EA0FCAEE33CA}">
+  <dimension ref="A1:D62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="58" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="47" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66" t="s">
+        <v>190</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="59"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="59"/>
+      <c r="B6" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>168</v>
+      </c>
+      <c r="D6" s="67" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="59"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="72" t="s">
+        <v>169</v>
+      </c>
+      <c r="D7" s="70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="59"/>
+      <c r="B8" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="47" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="59"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="71" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="59"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66" t="s">
+        <v>176</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="59"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="71" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="59"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="66" t="s">
+        <v>181</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="59"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="71" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="36" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="59"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="66" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="59"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="74" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="59"/>
+      <c r="B16" s="61" t="s">
+        <v>222</v>
+      </c>
+      <c r="C16" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="D16" s="75" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="59"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="59"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="66" t="s">
+        <v>195</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="59"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="59"/>
+      <c r="B20" s="62"/>
+      <c r="C20" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="59"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D21" s="36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="59"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="66" t="s">
+        <v>204</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="59"/>
+      <c r="B23" s="62"/>
+      <c r="C23" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" s="36" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="59"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="D24" s="67" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="59"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="59"/>
+      <c r="B26" s="62"/>
+      <c r="C26" s="66" t="s">
+        <v>216</v>
+      </c>
+      <c r="D26" s="44" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="59"/>
+      <c r="B27" s="62"/>
+      <c r="C27" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27" s="36" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="59"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="66" t="s">
+        <v>218</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="60"/>
+      <c r="B29" s="63"/>
+      <c r="C29" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="76"/>
+      <c r="B30" s="76"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="78"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="76"/>
+      <c r="B31" s="76"/>
+      <c r="C31" s="77"/>
+      <c r="D31" s="78"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="76"/>
+      <c r="B32" s="76"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="78"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="76"/>
+      <c r="B33" s="76"/>
+      <c r="C33" s="77"/>
+      <c r="D33" s="78"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="76"/>
+      <c r="B34" s="76"/>
+      <c r="C34" s="77"/>
+      <c r="D34" s="79"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="76"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="77"/>
+      <c r="D35" s="79"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="76"/>
+      <c r="B36" s="76"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="79"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="76"/>
+      <c r="B37" s="76"/>
+      <c r="C37" s="77"/>
+      <c r="D37" s="78"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="76"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="78"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="76"/>
+      <c r="B39" s="76"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="78"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="76"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="78"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="76"/>
+      <c r="B41" s="76"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="78"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="76"/>
+      <c r="B42" s="76"/>
+      <c r="C42" s="77"/>
+      <c r="D42" s="78"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="76"/>
+      <c r="B43" s="76"/>
+      <c r="C43" s="77"/>
+      <c r="D43" s="79"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="76"/>
+      <c r="B44" s="76"/>
+      <c r="C44" s="77"/>
+      <c r="D44" s="79"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="76"/>
+      <c r="B45" s="76"/>
+      <c r="C45" s="77"/>
+      <c r="D45" s="79"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="76"/>
+      <c r="B46" s="76"/>
+      <c r="C46" s="77"/>
+      <c r="D46" s="78"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="76"/>
+      <c r="B47" s="76"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="78"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="76"/>
+      <c r="B48" s="76"/>
+      <c r="C48" s="77"/>
+      <c r="D48" s="78"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="76"/>
+      <c r="B49" s="76"/>
+      <c r="C49" s="77"/>
+      <c r="D49" s="78"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="76"/>
+      <c r="B50" s="76"/>
+      <c r="C50" s="77"/>
+      <c r="D50" s="78"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="76"/>
+      <c r="B51" s="76"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="78"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="76"/>
+      <c r="B52" s="76"/>
+      <c r="C52" s="77"/>
+      <c r="D52" s="79"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="76"/>
+      <c r="B53" s="76"/>
+      <c r="C53" s="77"/>
+      <c r="D53" s="79"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="76"/>
+      <c r="B54" s="76"/>
+      <c r="C54" s="77"/>
+      <c r="D54" s="79"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="76"/>
+      <c r="B55" s="76"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="78"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="76"/>
+      <c r="B56" s="76"/>
+      <c r="C56" s="77"/>
+      <c r="D56" s="78"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="76"/>
+      <c r="B57" s="76"/>
+      <c r="C57" s="77"/>
+      <c r="D57" s="78"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="76"/>
+      <c r="B58" s="76"/>
+      <c r="C58" s="77"/>
+      <c r="D58" s="78"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="76"/>
+      <c r="B59" s="76"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="78"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="76"/>
+      <c r="B60" s="76"/>
+      <c r="C60" s="77"/>
+      <c r="D60" s="78"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="78"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="78"/>
+      <c r="D61" s="78"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="78"/>
+      <c r="B62" s="78"/>
+      <c r="C62" s="78"/>
+      <c r="D62" s="78"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B8:B15"/>
+    <mergeCell ref="B16:B29"/>
+    <mergeCell ref="A2:A29"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2483,6 +3282,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11c68bd7e868490b50c80001f2cf6c52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" xmlns:ns3="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7feae6b8f12256f9c4998c90aa2e28a" ns2:_="" ns3:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -2661,15 +3469,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
   <ds:schemaRefs>
@@ -2680,6 +3479,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2696,12 +3503,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added 10ms timer and general system requirements
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010371\Documents\GitHub\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB486B8-FAA2-443E-A152-94EFB772FD5D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A47CDE3-2718-4AE6-9499-2055BD9A120B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -215,13 +215,178 @@
   </si>
   <si>
     <t>TDC_FSM_03</t>
+  </si>
+  <si>
+    <t>The module shall set o_count to "000000000000000000000000" if i_reset_n = '0'</t>
+  </si>
+  <si>
+    <t>The module shall have an asynchronous reset via i_reset_n</t>
+  </si>
+  <si>
+    <t>The module shall not use i_countenb but have as dummy input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall not use i_countinit but have as dummy input </t>
+  </si>
+  <si>
+    <t>The module shall roll over (set) o_count[3:0] back to "0000" when o_count[3:0] = "1001" and i_reset_n /='0' and i_latchcount = '1'</t>
+  </si>
+  <si>
+    <t>The module shall roll over (set)  o_count[7:4] back to "0000" when o_count[7:4]= "1001" and i_reset_n /='0' and i_latchcount = '1'</t>
+  </si>
+  <si>
+    <t>The module shall roll (set) over 0_count[11:8] back to "0000" when o_count[11:8] = "1001" and i_reset_n /='0' and i_latchcount = '1'</t>
+  </si>
+  <si>
+    <t>The module shall roll (set) over o_count[15:12] back to "0000" when o_count[15:12] = "1001" and i_reset_n /='0' and i_latchcount = '1'</t>
+  </si>
+  <si>
+    <t>The module shall roll (set) over o_count[19:16] back to "0000" when o_count[19:16] = "1001" and i_reset_n /='0' and i_latchcount = '1'</t>
+  </si>
+  <si>
+    <t>The module shall roll (set) over o_count[23:20] back to "0000" when o_count[23:20] = "0110" and i_reset_n /='0' and i_latchcount = '1'</t>
+  </si>
+  <si>
+    <t>The module shall not change o_count if i_latchcount = '0' and i_reset_n = '1'</t>
+  </si>
+  <si>
+    <t>Roll Over</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The module shall represent the MM:SS:mm timer in BCD on o_count with o_count[3:0] corresponding to the hundreths of a second place, o_count[7:4] the tenths of a second place and so on.  </t>
+  </si>
+  <si>
+    <t>Increment</t>
+  </si>
+  <si>
+    <t>The module shall increment the MM:SS:mm timer in BCD on o_count every rising edge of i_rtcclk if i_reset_n='1' and i_latchcount='1'  unless o_count is due to roll over to "000000000000000000000000"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BCD </t>
+  </si>
+  <si>
+    <t>BCD_INIT_01</t>
+  </si>
+  <si>
+    <t>BCD_INIT_02</t>
+  </si>
+  <si>
+    <t>BCD_INIT_03</t>
+  </si>
+  <si>
+    <t>BCD_INIT_04</t>
+  </si>
+  <si>
+    <t>BCD_RO_01</t>
+  </si>
+  <si>
+    <t>BCD_RO_02</t>
+  </si>
+  <si>
+    <t>BCD_RO_03</t>
+  </si>
+  <si>
+    <t>BCD_RO_04</t>
+  </si>
+  <si>
+    <t>BCD_RO_05</t>
+  </si>
+  <si>
+    <t>BCD_RO_06</t>
+  </si>
+  <si>
+    <t>BCD_INC_01</t>
+  </si>
+  <si>
+    <t>BCD_INC_02</t>
+  </si>
+  <si>
+    <t>BCD_INC_03</t>
+  </si>
+  <si>
+    <t>TIMER</t>
+  </si>
+  <si>
+    <t>TIMER_INIT_01</t>
+  </si>
+  <si>
+    <t>Upon initialization module shall set count to value of 0.</t>
+  </si>
+  <si>
+    <t>TIMER_INIT_02</t>
+  </si>
+  <si>
+    <t>Upon initialization module shall set base_tick output to logic low.</t>
+  </si>
+  <si>
+    <t>Counting</t>
+  </si>
+  <si>
+    <t>TIMER_CNT_01</t>
+  </si>
+  <si>
+    <t>Module shall increment count on every positive edge of 100MHz SYS_CLK input when enable is high.</t>
+  </si>
+  <si>
+    <t>TIMER_CNT_02</t>
+  </si>
+  <si>
+    <t>Module shall invert base_tick output once count equals 1000000 / 2</t>
+  </si>
+  <si>
+    <t>Reset</t>
+  </si>
+  <si>
+    <t>TIMER_RST_01</t>
+  </si>
+  <si>
+    <t>Module shall set count to value of 0 when system reset input is logic low.</t>
+  </si>
+  <si>
+    <t>TOP</t>
+  </si>
+  <si>
+    <t>TOP_INIT_01</t>
+  </si>
+  <si>
+    <t>Upon initialization toggle RST_N active low to trigger system reset</t>
+  </si>
+  <si>
+    <t>Clocking</t>
+  </si>
+  <si>
+    <t>TOP_CLK_01</t>
+  </si>
+  <si>
+    <t>Module shall receive 100MHz Xilinx Artix-7 clock to use as SYS_CLK</t>
+  </si>
+  <si>
+    <t>Module Instantiation</t>
+  </si>
+  <si>
+    <t>TOP_INST_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module shall pass SYS_CLK and RST_N to Trigger Detection, 10ms Timer, BCD to 7-Seg and 7-Seg module instantiations </t>
+  </si>
+  <si>
+    <t>TOP_INST_02</t>
+  </si>
+  <si>
+    <t>Module shall pass only RST_N to 20-bit Counter</t>
+  </si>
+  <si>
+    <t>TOP_RST_01</t>
+  </si>
+  <si>
+    <t>Module shall update RST_N asynchronously</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,8 +407,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,8 +434,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEDEDED"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="30">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -632,11 +822,260 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -715,6 +1154,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -730,6 +1177,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -739,8 +1195,66 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1055,19 +1569,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26B4EAFD-D6BC-4B33-AEA7-1FB008F58338}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="124.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="124.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="29" t="s">
         <v>2</v>
       </c>
@@ -1081,11 +1595,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="25" t="s">
@@ -1095,9 +1609,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
       <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1105,9 +1619,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="43"/>
+      <c r="B4" s="43"/>
       <c r="C4" s="9" t="s">
         <v>43</v>
       </c>
@@ -1115,9 +1629,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="35"/>
-      <c r="B5" s="35"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="43"/>
+      <c r="B5" s="43"/>
       <c r="C5" s="13" t="s">
         <v>44</v>
       </c>
@@ -1125,9 +1639,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="43"/>
+      <c r="B6" s="44"/>
       <c r="C6" s="32" t="s">
         <v>45</v>
       </c>
@@ -1135,9 +1649,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
+      <c r="B7" s="43" t="s">
         <v>32</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -1147,9 +1661,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="23" t="s">
         <v>34</v>
       </c>
@@ -1157,9 +1671,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="43"/>
+      <c r="B9" s="43"/>
       <c r="C9" s="15" t="s">
         <v>59</v>
       </c>
@@ -1167,9 +1681,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
-      <c r="B10" s="35"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="43"/>
+      <c r="B10" s="43"/>
       <c r="C10" s="23" t="s">
         <v>35</v>
       </c>
@@ -1177,9 +1691,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="35"/>
-      <c r="B11" s="38"/>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="43"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="17" t="s">
         <v>36</v>
       </c>
@@ -1187,9 +1701,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
-      <c r="B12" s="34" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="43"/>
+      <c r="B12" s="42" t="s">
         <v>37</v>
       </c>
       <c r="C12" s="27" t="s">
@@ -1199,9 +1713,9 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="43"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="19" t="s">
         <v>39</v>
       </c>
@@ -1209,9 +1723,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="43"/>
+      <c r="B14" s="43"/>
       <c r="C14" s="23" t="s">
         <v>40</v>
       </c>
@@ -1219,9 +1733,9 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
       <c r="C15" s="21" t="s">
         <v>46</v>
       </c>
@@ -1229,44 +1743,44 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22"/>
       <c r="D22"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23"/>
       <c r="D23"/>
     </row>
@@ -1283,47 +1797,280 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B832A1-37E9-4B2E-807C-B34D7E444DA2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="89.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="66"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="66"/>
+      <c r="B4" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>95</v>
+      </c>
+      <c r="D4" s="58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="66"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="60" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="67"/>
+      <c r="B6" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA2C20F1-AFF3-4389-955F-F90E6A0B5D40}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" customWidth="1"/>
+    <col min="4" max="4" width="154.140625" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="34" t="s">
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="48"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="48"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="48"/>
+      <c r="B6" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="48"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="48"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="48"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="48"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="48"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="48"/>
+      <c r="B12" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A2:A14"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1336,16 +2083,16 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1359,11 +2106,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="50" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -1373,9 +2120,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="40"/>
+      <c r="B3" s="51"/>
       <c r="C3" s="4" t="s">
         <v>20</v>
       </c>
@@ -1383,8 +2130,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="51"/>
       <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
@@ -1392,8 +2139,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="40"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="51"/>
       <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
@@ -1401,8 +2148,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B6" s="40"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="51"/>
       <c r="C6" s="4" t="s">
         <v>23</v>
       </c>
@@ -1410,8 +2157,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" s="40"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="51"/>
       <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
@@ -1419,8 +2166,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="40"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="51"/>
       <c r="C8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1428,8 +2175,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B9" s="40"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="51"/>
       <c r="C9" s="4" t="s">
         <v>26</v>
       </c>
@@ -1437,8 +2184,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B10" s="40"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" s="51"/>
       <c r="C10" s="4" t="s">
         <v>27</v>
       </c>
@@ -1446,8 +2193,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="41"/>
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="52"/>
       <c r="C11" s="8" t="s">
         <v>28</v>
       </c>
@@ -1455,7 +2202,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -1475,17 +2222,119 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="102.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="74" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="72"/>
+      <c r="B3" s="56" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>106</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="72"/>
+      <c r="B4" s="72" t="s">
+        <v>108</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="72"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="70" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="72"/>
+      <c r="B6" s="73" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="75" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010008B8F660E2FD5A4F9C25F557691C2E7B" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="11c68bd7e868490b50c80001f2cf6c52">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fe6e073-fbcf-4c9f-9467-c4294a786ad2" xmlns:ns3="b6b24143-0de2-4c5a-b05e-2e6859d8ef3d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f7feae6b8f12256f9c4998c90aa2e28a" ns2:_="" ns3:_="">
     <xsd:import namespace="0fe6e073-fbcf-4c9f-9467-c4294a786ad2"/>
@@ -1664,22 +2513,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D06D32E1-CC4E-4E18-B835-24ECDC821600}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1696,21 +2547,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A63DF73E-DD3D-41FF-8D79-2B1DF9FB0290}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D428352-D980-4D82-A5A0-02B72263C90B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed naming conventions for timer module but not for Top level module
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A47CDE3-2718-4AE6-9499-2055BD9A120B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B3B140-452C-4DEE-9037-8982028587DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="4" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
@@ -310,15 +310,9 @@
     <t>TIMER_INIT_01</t>
   </si>
   <si>
-    <t>Upon initialization module shall set count to value of 0.</t>
-  </si>
-  <si>
     <t>TIMER_INIT_02</t>
   </si>
   <si>
-    <t>Upon initialization module shall set base_tick output to logic low.</t>
-  </si>
-  <si>
     <t>Counting</t>
   </si>
   <si>
@@ -380,6 +374,12 @@
   </si>
   <si>
     <t>Module shall update RST_N asynchronously</t>
+  </si>
+  <si>
+    <t>Module shall set count to value of 0 when i_reset_n is logic low.</t>
+  </si>
+  <si>
+    <t>Module shall set base_tick logic low when i_reset_n is logic low.</t>
   </si>
 </sst>
 </file>
@@ -1799,8 +1799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B832A1-37E9-4B2E-807C-B34D7E444DA2}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,51 +1836,51 @@
         <v>90</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="66"/>
       <c r="B3" s="69"/>
       <c r="C3" s="59" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="60" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="66"/>
       <c r="B4" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="58" t="s">
         <v>94</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="66"/>
       <c r="B5" s="69"/>
       <c r="C5" s="61" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D5" s="60" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="67"/>
       <c r="B6" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="64" t="s">
         <v>99</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2222,10 +2222,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,67 +2252,73 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="71" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2" s="56" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="74" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="72"/>
       <c r="B3" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="70" t="s">
         <v>105</v>
-      </c>
-      <c r="C3" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="70" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="72"/>
       <c r="B4" s="72" t="s">
+        <v>106</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>107</v>
+      </c>
+      <c r="D4" s="74" t="s">
         <v>108</v>
-      </c>
-      <c r="C4" s="74" t="s">
-        <v>109</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="72"/>
       <c r="B5" s="72"/>
       <c r="C5" s="70" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D5" s="70" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="72"/>
-      <c r="B6" s="73" t="s">
-        <v>99</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" s="75" t="s">
-        <v>114</v>
+      <c r="B6" s="56"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="70"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="72"/>
+      <c r="B7" s="73" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A2:A7"/>
     <mergeCell ref="B4:B5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added hardware input requirement for Top module
</commit_message>
<xml_diff>
--- a/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
+++ b/Life_Cycle_Data/Requirements_Docs/Verilog Stopwatch Requirments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\training\stopwatch\Verilog_Stopwatch\Life_Cycle_Data\Requirements_Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B3B140-452C-4DEE-9037-8982028587DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA3CB07-F97C-47B2-A17A-2B206BF48E94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-5340" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{CD9692A4-B00F-4694-A4FD-38B7C9FAA45F}"/>
   </bookViews>
   <sheets>
     <sheet name="Trigger Detection Circuit" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="121">
   <si>
     <t>Requirement Tag</t>
   </si>
@@ -319,33 +319,21 @@
     <t>TIMER_CNT_01</t>
   </si>
   <si>
-    <t>Module shall increment count on every positive edge of 100MHz SYS_CLK input when enable is high.</t>
-  </si>
-  <si>
     <t>TIMER_CNT_02</t>
   </si>
   <si>
-    <t>Module shall invert base_tick output once count equals 1000000 / 2</t>
-  </si>
-  <si>
     <t>Reset</t>
   </si>
   <si>
     <t>TIMER_RST_01</t>
   </si>
   <si>
-    <t>Module shall set count to value of 0 when system reset input is logic low.</t>
-  </si>
-  <si>
     <t>TOP</t>
   </si>
   <si>
     <t>TOP_INIT_01</t>
   </si>
   <si>
-    <t>Upon initialization toggle RST_N active low to trigger system reset</t>
-  </si>
-  <si>
     <t>Clocking</t>
   </si>
   <si>
@@ -379,7 +367,37 @@
     <t>Module shall set count to value of 0 when i_reset_n is logic low.</t>
   </si>
   <si>
-    <t>Module shall set base_tick logic low when i_reset_n is logic low.</t>
+    <t>Module shall invert o_basetick output once count equals 1000000 / 2</t>
+  </si>
+  <si>
+    <t>Module shall set o_basetick logic low when i_reset_n is logic low.</t>
+  </si>
+  <si>
+    <t>Module shall increment count on every positive edge of 100MHz i_sclk input when i_timerenb is high.</t>
+  </si>
+  <si>
+    <t>Module shall set internal counter to value of 0 when system reset input is logic low.</t>
+  </si>
+  <si>
+    <t>Module shall toggle RST_N logic low to trigger system reset</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>TOP_OUT_01</t>
+  </si>
+  <si>
+    <t>Module shall display out current state of stopwatch system</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>TOP_IN_01</t>
+  </si>
+  <si>
+    <t>Module shall use FPGA hardware pushbutton as input to Trigger Detection module</t>
   </si>
 </sst>
 </file>
@@ -447,7 +465,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -894,57 +912,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -952,26 +921,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -982,34 +951,17 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -1017,14 +969,55 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -1036,33 +1029,132 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -1075,7 +1167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1195,63 +1287,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -1570,7 +1692,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,10 +1919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64B832A1-37E9-4B2E-807C-B34D7E444DA2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,80 +1930,83 @@
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="31.28515625" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="89.85546875" customWidth="1"/>
+    <col min="4" max="4" width="92.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="63" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="58" t="s">
+      <c r="D2" s="65" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="66" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="59"/>
+      <c r="B4" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="64" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="65" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="59"/>
+      <c r="B5" s="60"/>
+      <c r="C5" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="70" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="68"/>
+      <c r="B6" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="73" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
-      <c r="B4" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="61" t="s">
-        <v>95</v>
-      </c>
-      <c r="D5" s="60" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="67"/>
-      <c r="B6" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" s="64" t="s">
-        <v>99</v>
-      </c>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D9" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2222,10 +2347,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5643AF75-7382-4467-A67F-D3A6F4BA857E}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2233,93 +2358,111 @@
     <col min="1" max="1" width="34.85546875" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="4" max="4" width="102.85546875" customWidth="1"/>
+    <col min="4" max="4" width="104.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="63" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="80" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="76"/>
+      <c r="B3" s="81" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="81" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="74" t="s">
+      <c r="D3" s="78" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="74" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="76"/>
+      <c r="B4" s="81" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="85" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="79" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="76"/>
+      <c r="B5" s="82" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="72"/>
-      <c r="B3" s="56" t="s">
+      <c r="C5" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="D5" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="70" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="76"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="85" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="72"/>
-      <c r="B4" s="72" t="s">
+      <c r="D6" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="74" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="76"/>
+      <c r="B7" s="81" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="68"/>
+      <c r="B8" s="83" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D8" s="87" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="72"/>
-      <c r="B5" s="72"/>
-      <c r="C5" s="70" t="s">
-        <v>109</v>
-      </c>
-      <c r="D5" s="70" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="72"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="72"/>
-      <c r="B7" s="73" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="75" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="75" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>